<commit_message>
Save last stable rank
</commit_message>
<xml_diff>
--- a/ranks.xlsx
+++ b/ranks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uf430mri\mk-rank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADA6043-3B9B-4F09-99EC-F566FDF0B14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D5949E-2480-4375-A9D6-07A92085C92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,10 +625,10 @@
         <v>30</v>
       </c>
       <c r="C2">
-        <v>1049</v>
+        <v>1037</v>
       </c>
       <c r="D2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>1000</v>
@@ -681,10 +681,10 @@
         <v>31</v>
       </c>
       <c r="C3">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>1000</v>
@@ -731,10 +731,10 @@
         <v>32</v>
       </c>
       <c r="C4">
-        <v>1167</v>
+        <v>1176</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>1000</v>
@@ -823,10 +823,10 @@
         <v>33</v>
       </c>
       <c r="C5">
-        <v>891</v>
+        <v>896</v>
       </c>
       <c r="D5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>1000</v>

</xml_diff>